<commit_message>
str, var, rust_vs_cpp modifie
</commit_message>
<xml_diff>
--- a/rust_vs_cpp.xlsx
+++ b/rust_vs_cpp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhi3700/F/coding/github_repos/My_Learning-Rust/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092C36FC-02BD-4F4A-B3D3-700DF2EE158E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EFFF23-5E58-D54E-B38A-C0BCA57FF5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14420" xr2:uid="{883BD0E7-27B8-E043-8844-C2809D0A594F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Rust</t>
   </si>
@@ -140,13 +140,64 @@
     x + 5        // M-1
     return x + 5;    // M-2
 }</t>
+  </si>
+  <si>
+    <t>impl Animal for Sheep</t>
+  </si>
+  <si>
+    <t>class Sheep is Animal</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>char/string</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>convert into string</t>
+  </si>
+  <si>
+    <t>define var</t>
+  </si>
+  <si>
+    <t>const pointer vs shared references</t>
+  </si>
+  <si>
+    <t>non-const pointer vs mutable references</t>
+  </si>
+  <si>
+    <t>switch/match</t>
+  </si>
+  <si>
+    <t>if condition</t>
+  </si>
+  <si>
+    <t>for loop</t>
+  </si>
+  <si>
+    <t>while loop</t>
+  </si>
+  <si>
+    <t>do-while loop</t>
+  </si>
+  <si>
+    <t>ternary operator</t>
+  </si>
+  <si>
+    <t>return value</t>
+  </si>
+  <si>
+    <t>Inheritance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -162,8 +213,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +237,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -221,11 +285,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,129 +608,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C028A04-14AA-A248-B03C-E0E17A6163FF}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="30.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="48.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rust references, dereferences ownership done
</commit_message>
<xml_diff>
--- a/rust_vs_cpp.xlsx
+++ b/rust_vs_cpp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhi3700/F/coding/github_repos/My_Learning-Rust/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EFFF23-5E58-D54E-B38A-C0BCA57FF5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9501CF51-F66A-5E48-9CC4-5C01567946F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14420" xr2:uid="{883BD0E7-27B8-E043-8844-C2809D0A594F}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14400" xr2:uid="{883BD0E7-27B8-E043-8844-C2809D0A594F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Rust</t>
   </si>
@@ -191,6 +191,23 @@
   </si>
   <si>
     <t>Inheritance</t>
+  </si>
+  <si>
+    <t>Borrowing or Referencing</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Dereferencing</t>
+  </si>
+  <si>
+    <t>*
+Automatically gets dereferenced in case of reference to a reference. No need to write like this **. Instead just use *.
+Follow this file - "./tuts/ownership/dereference_2.rs"</t>
   </si>
 </sst>
 </file>
@@ -608,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C028A04-14AA-A248-B03C-E0E17A6163FF}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -787,6 +804,28 @@
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Calculator App added, arg added, rust_vs_cpp updated with option, result analogy
</commit_message>
<xml_diff>
--- a/rust_vs_cpp.xlsx
+++ b/rust_vs_cpp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhi3700/F/coding/github_repos/My_Learning-Rust/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9501CF51-F66A-5E48-9CC4-5C01567946F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DA12FD-6AA5-354E-9C23-1B3E030F60C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14400" xr2:uid="{883BD0E7-27B8-E043-8844-C2809D0A594F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Rust</t>
   </si>
@@ -208,13 +208,55 @@
     <t>*
 Automatically gets dereferenced in case of reference to a reference. No need to write like this **. Instead just use *.
 Follow this file - "./tuts/ownership/dereference_2.rs"</t>
+  </si>
+  <si>
+    <t>Optional &amp; Result</t>
+  </si>
+  <si>
+    <t>std::optional,
+std::expected</t>
+  </si>
+  <si>
+    <t>Option {
+  Some,
+  None
+}
+Result {
+  Ok
+  Err
+}</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Example:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://gist.github.com/L0N3W0LF/c9f6e7bb4df1883b147e3c846968468a </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,14 +273,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +324,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -308,7 +378,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -625,21 +704,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C028A04-14AA-A248-B03C-E0E17A6163FF}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="57" style="8" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="48.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -649,9 +729,12 @@
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -660,9 +743,10 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -671,9 +755,10 @@
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -682,9 +767,10 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -693,9 +779,10 @@
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -704,9 +791,10 @@
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -715,9 +803,10 @@
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -726,9 +815,10 @@
       <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -737,9 +827,10 @@
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -748,9 +839,10 @@
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -759,9 +851,10 @@
       <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -770,9 +863,10 @@
       <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -781,9 +875,10 @@
       <c r="C13" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -792,9 +887,10 @@
       <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -803,9 +899,10 @@
       <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -814,9 +911,10 @@
       <c r="C16" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -824,6 +922,21 @@
       </c>
       <c r="C17" s="3" t="s">
         <v>48</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>